<commit_message>
Spojene staty for USA
</commit_message>
<xml_diff>
--- a/Predatori_data.xlsx
+++ b/Predatori_data.xlsx
@@ -2767,9 +2767,6 @@
     <t>nezařazeno</t>
   </si>
   <si>
-    <t>Spojené státy</t>
-  </si>
-  <si>
     <t>Bulharsko</t>
   </si>
   <si>
@@ -2858,6 +2855,9 @@
   </si>
   <si>
     <t>Ázerbajdžán</t>
+  </si>
+  <si>
+    <t>USA</t>
   </si>
 </sst>
 </file>
@@ -3220,10 +3220,10 @@
   <dimension ref="A1:O405"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D19" sqref="D19"/>
+      <selection pane="bottomRight" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3306,7 +3306,7 @@
         <v>312</v>
       </c>
       <c r="E2" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F2" t="s">
         <v>257</v>
@@ -3353,7 +3353,7 @@
         <v>312</v>
       </c>
       <c r="E3" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F3" t="s">
         <v>257</v>
@@ -3380,7 +3380,7 @@
         <v>312</v>
       </c>
       <c r="E4" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F4" t="s">
         <v>257</v>
@@ -3427,7 +3427,7 @@
         <v>312</v>
       </c>
       <c r="E5" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F5" t="s">
         <v>257</v>
@@ -3474,7 +3474,7 @@
         <v>312</v>
       </c>
       <c r="E6" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F6" t="s">
         <v>257</v>
@@ -3521,7 +3521,7 @@
         <v>344</v>
       </c>
       <c r="E7" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F7" t="s">
         <v>257</v>
@@ -3568,7 +3568,7 @@
         <v>344</v>
       </c>
       <c r="E8" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F8" t="s">
         <v>257</v>
@@ -3595,7 +3595,7 @@
         <v>331</v>
       </c>
       <c r="E9" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="F9" t="s">
         <v>257</v>
@@ -3642,7 +3642,7 @@
         <v>543</v>
       </c>
       <c r="E10" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="F10" t="s">
         <v>257</v>
@@ -3669,7 +3669,7 @@
         <v>546</v>
       </c>
       <c r="E11" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="F11" t="s">
         <v>257</v>
@@ -3696,7 +3696,7 @@
         <v>546</v>
       </c>
       <c r="E12" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="F12" t="s">
         <v>257</v>
@@ -3723,7 +3723,7 @@
         <v>546</v>
       </c>
       <c r="E13" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="F13" t="s">
         <v>257</v>
@@ -3750,7 +3750,7 @@
         <v>546</v>
       </c>
       <c r="E14" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="F14" t="s">
         <v>257</v>
@@ -3777,7 +3777,7 @@
         <v>263</v>
       </c>
       <c r="E15" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="F15" t="s">
         <v>261</v>
@@ -3824,7 +3824,7 @@
         <v>518</v>
       </c>
       <c r="E16" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F16" t="s">
         <v>257</v>
@@ -3871,7 +3871,7 @@
         <v>905</v>
       </c>
       <c r="E17" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="F17" t="s">
         <v>261</v>
@@ -3918,7 +3918,7 @@
         <v>354</v>
       </c>
       <c r="E18" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F18" t="s">
         <v>257</v>
@@ -3965,7 +3965,7 @@
         <v>354</v>
       </c>
       <c r="E19" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F19" t="s">
         <v>257</v>
@@ -4012,7 +4012,7 @@
         <v>354</v>
       </c>
       <c r="E20" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F20" t="s">
         <v>257</v>
@@ -4059,7 +4059,7 @@
         <v>354</v>
       </c>
       <c r="E21" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F21" t="s">
         <v>257</v>
@@ -4106,7 +4106,7 @@
         <v>370</v>
       </c>
       <c r="E22" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F22" t="s">
         <v>257</v>
@@ -4153,7 +4153,7 @@
         <v>504</v>
       </c>
       <c r="E23" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F23" t="s">
         <v>257</v>
@@ -4180,7 +4180,7 @@
         <v>504</v>
       </c>
       <c r="E24" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F24" t="s">
         <v>257</v>
@@ -4207,7 +4207,7 @@
         <v>504</v>
       </c>
       <c r="E25" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F25" t="s">
         <v>257</v>
@@ -4234,7 +4234,7 @@
         <v>370</v>
       </c>
       <c r="E26" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F26" t="s">
         <v>257</v>
@@ -4281,7 +4281,7 @@
         <v>354</v>
       </c>
       <c r="E27" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F27" t="s">
         <v>257</v>
@@ -4308,7 +4308,7 @@
         <v>354</v>
       </c>
       <c r="E28" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F28" t="s">
         <v>257</v>
@@ -4355,7 +4355,7 @@
         <v>370</v>
       </c>
       <c r="E29" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F29" t="s">
         <v>257</v>
@@ -4402,7 +4402,7 @@
         <v>354</v>
       </c>
       <c r="E30" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F30" t="s">
         <v>257</v>
@@ -4449,7 +4449,7 @@
         <v>354</v>
       </c>
       <c r="E31" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F31" t="s">
         <v>257</v>
@@ -4496,7 +4496,7 @@
         <v>504</v>
       </c>
       <c r="E32" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F32" t="s">
         <v>257</v>
@@ -4523,7 +4523,7 @@
         <v>504</v>
       </c>
       <c r="E33" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F33" t="s">
         <v>257</v>
@@ -4550,7 +4550,7 @@
         <v>354</v>
       </c>
       <c r="E34" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F34" t="s">
         <v>257</v>
@@ -4597,7 +4597,7 @@
         <v>370</v>
       </c>
       <c r="E35" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F35" t="s">
         <v>257</v>
@@ -4624,7 +4624,7 @@
         <v>504</v>
       </c>
       <c r="E36" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F36" t="s">
         <v>257</v>
@@ -4651,7 +4651,7 @@
         <v>504</v>
       </c>
       <c r="E37" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F37" t="s">
         <v>257</v>
@@ -4698,7 +4698,7 @@
         <v>331</v>
       </c>
       <c r="E38" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="F38" t="s">
         <v>257</v>
@@ -4745,7 +4745,7 @@
         <v>564</v>
       </c>
       <c r="E39" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="F39" t="s">
         <v>257</v>
@@ -4792,7 +4792,7 @@
         <v>269</v>
       </c>
       <c r="E40" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="F40" t="s">
         <v>261</v>
@@ -4839,7 +4839,7 @@
         <v>407</v>
       </c>
       <c r="E41" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="F41" t="s">
         <v>257</v>
@@ -4886,7 +4886,7 @@
         <v>898</v>
       </c>
       <c r="E42" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="F42" t="s">
         <v>261</v>
@@ -4913,7 +4913,7 @@
         <v>557</v>
       </c>
       <c r="E43" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="F43" t="s">
         <v>261</v>
@@ -4960,7 +4960,7 @@
         <v>494</v>
       </c>
       <c r="E44" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="F44" t="s">
         <v>257</v>
@@ -5007,7 +5007,7 @@
         <v>866</v>
       </c>
       <c r="E45" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="F45" t="s">
         <v>261</v>
@@ -5034,7 +5034,7 @@
         <v>275</v>
       </c>
       <c r="E46" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="F46" t="s">
         <v>261</v>
@@ -5081,7 +5081,7 @@
         <v>275</v>
       </c>
       <c r="E47" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="F47" t="s">
         <v>261</v>
@@ -5128,7 +5128,7 @@
         <v>282</v>
       </c>
       <c r="E48" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="F48" t="s">
         <v>257</v>
@@ -5175,7 +5175,7 @@
         <v>567</v>
       </c>
       <c r="E49" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="F49" t="s">
         <v>261</v>
@@ -5222,7 +5222,7 @@
         <v>419</v>
       </c>
       <c r="E50" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F50" t="s">
         <v>257</v>
@@ -5269,7 +5269,7 @@
         <v>331</v>
       </c>
       <c r="E51" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="F51" t="s">
         <v>257</v>
@@ -5316,7 +5316,7 @@
         <v>410</v>
       </c>
       <c r="E52" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="F52" t="s">
         <v>257</v>
@@ -5363,7 +5363,7 @@
         <v>410</v>
       </c>
       <c r="E53" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="F53" t="s">
         <v>257</v>
@@ -5410,7 +5410,7 @@
         <v>370</v>
       </c>
       <c r="E54" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F54" t="s">
         <v>257</v>
@@ -5437,7 +5437,7 @@
         <v>295</v>
       </c>
       <c r="E55" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="F55" t="s">
         <v>257</v>
@@ -5484,7 +5484,7 @@
         <v>295</v>
       </c>
       <c r="E56" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="F56" t="s">
         <v>257</v>
@@ -5531,7 +5531,7 @@
         <v>546</v>
       </c>
       <c r="E57" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="F57" t="s">
         <v>257</v>
@@ -5558,7 +5558,7 @@
         <v>313</v>
       </c>
       <c r="E58" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F58" t="s">
         <v>261</v>
@@ -5605,7 +5605,7 @@
         <v>494</v>
       </c>
       <c r="E59" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="F59" t="s">
         <v>257</v>
@@ -5652,7 +5652,7 @@
         <v>312</v>
       </c>
       <c r="E60" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F60" t="s">
         <v>257</v>
@@ -5679,7 +5679,7 @@
         <v>464</v>
       </c>
       <c r="E61" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="F61" t="s">
         <v>261</v>
@@ -5726,7 +5726,7 @@
         <v>736</v>
       </c>
       <c r="E62" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="F62" t="s">
         <v>257</v>
@@ -5753,7 +5753,7 @@
         <v>380</v>
       </c>
       <c r="E63" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="F63" t="s">
         <v>257</v>
@@ -5800,7 +5800,7 @@
         <v>380</v>
       </c>
       <c r="E64" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="F64" t="s">
         <v>257</v>
@@ -5847,7 +5847,7 @@
         <v>380</v>
       </c>
       <c r="E65" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="F65" t="s">
         <v>257</v>
@@ -5874,7 +5874,7 @@
         <v>513</v>
       </c>
       <c r="E66" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F66" t="s">
         <v>257</v>
@@ -5921,7 +5921,7 @@
         <v>513</v>
       </c>
       <c r="E67" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F67" t="s">
         <v>257</v>
@@ -5968,7 +5968,7 @@
         <v>380</v>
       </c>
       <c r="E68" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="F68" t="s">
         <v>257</v>
@@ -6015,7 +6015,7 @@
         <v>380</v>
       </c>
       <c r="E69" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="F69" t="s">
         <v>257</v>
@@ -6062,7 +6062,7 @@
         <v>380</v>
       </c>
       <c r="E70" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="F70" t="s">
         <v>257</v>
@@ -6089,7 +6089,7 @@
         <v>380</v>
       </c>
       <c r="E71" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="F71" t="s">
         <v>257</v>
@@ -6136,7 +6136,7 @@
         <v>380</v>
       </c>
       <c r="E72" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="F72" t="s">
         <v>257</v>
@@ -6183,7 +6183,7 @@
         <v>380</v>
       </c>
       <c r="E73" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="F73" t="s">
         <v>257</v>
@@ -6210,7 +6210,7 @@
         <v>380</v>
       </c>
       <c r="E74" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="F74" t="s">
         <v>257</v>
@@ -6257,7 +6257,7 @@
         <v>380</v>
       </c>
       <c r="E75" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="F75" t="s">
         <v>257</v>
@@ -6304,7 +6304,7 @@
         <v>380</v>
       </c>
       <c r="E76" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="F76" t="s">
         <v>257</v>
@@ -6351,7 +6351,7 @@
         <v>380</v>
       </c>
       <c r="E77" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="F77" t="s">
         <v>257</v>
@@ -6398,7 +6398,7 @@
         <v>380</v>
       </c>
       <c r="E78" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="F78" t="s">
         <v>257</v>
@@ -6445,7 +6445,7 @@
         <v>380</v>
       </c>
       <c r="E79" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="F79" t="s">
         <v>257</v>
@@ -6492,7 +6492,7 @@
         <v>380</v>
       </c>
       <c r="E80" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="F80" t="s">
         <v>257</v>
@@ -6539,7 +6539,7 @@
         <v>380</v>
       </c>
       <c r="E81" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="F81" t="s">
         <v>257</v>
@@ -6586,7 +6586,7 @@
         <v>380</v>
       </c>
       <c r="E82" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="F82" t="s">
         <v>257</v>
@@ -6613,7 +6613,7 @@
         <v>380</v>
       </c>
       <c r="E83" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="F83" t="s">
         <v>257</v>
@@ -6660,7 +6660,7 @@
         <v>380</v>
       </c>
       <c r="E84" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="F84" t="s">
         <v>257</v>
@@ -6707,7 +6707,7 @@
         <v>380</v>
       </c>
       <c r="E85" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="F85" t="s">
         <v>257</v>
@@ -6754,7 +6754,7 @@
         <v>380</v>
       </c>
       <c r="E86" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="F86" t="s">
         <v>257</v>
@@ -6801,7 +6801,7 @@
         <v>380</v>
       </c>
       <c r="E87" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="F87" t="s">
         <v>257</v>
@@ -6848,7 +6848,7 @@
         <v>380</v>
       </c>
       <c r="E88" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="F88" t="s">
         <v>257</v>
@@ -6895,7 +6895,7 @@
         <v>380</v>
       </c>
       <c r="E89" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="F89" t="s">
         <v>257</v>
@@ -6942,7 +6942,7 @@
         <v>380</v>
       </c>
       <c r="E90" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="F90" t="s">
         <v>257</v>
@@ -6989,7 +6989,7 @@
         <v>380</v>
       </c>
       <c r="E91" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="F91" t="s">
         <v>257</v>
@@ -7036,7 +7036,7 @@
         <v>380</v>
       </c>
       <c r="E92" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="F92" t="s">
         <v>257</v>
@@ -7083,7 +7083,7 @@
         <v>380</v>
       </c>
       <c r="E93" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="F93" t="s">
         <v>257</v>
@@ -7130,7 +7130,7 @@
         <v>380</v>
       </c>
       <c r="E94" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="F94" t="s">
         <v>257</v>
@@ -7177,7 +7177,7 @@
         <v>380</v>
       </c>
       <c r="E95" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="F95" t="s">
         <v>257</v>
@@ -7224,7 +7224,7 @@
         <v>518</v>
       </c>
       <c r="E96" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F96" t="s">
         <v>257</v>
@@ -7271,7 +7271,7 @@
         <v>494</v>
       </c>
       <c r="E97" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="F97" t="s">
         <v>257</v>
@@ -7318,7 +7318,7 @@
         <v>277</v>
       </c>
       <c r="E98" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="F98" t="s">
         <v>257</v>
@@ -7365,7 +7365,7 @@
         <v>452</v>
       </c>
       <c r="E99" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="F99" t="s">
         <v>257</v>
@@ -7412,7 +7412,7 @@
         <v>286</v>
       </c>
       <c r="E100" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="F100" t="s">
         <v>257</v>
@@ -7459,7 +7459,7 @@
         <v>338</v>
       </c>
       <c r="E101" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="F101" t="s">
         <v>257</v>
@@ -7506,7 +7506,7 @@
         <v>336</v>
       </c>
       <c r="E102" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="F102" t="s">
         <v>261</v>
@@ -7553,7 +7553,7 @@
         <v>312</v>
       </c>
       <c r="E103" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F103" t="s">
         <v>257</v>
@@ -7600,7 +7600,7 @@
         <v>407</v>
       </c>
       <c r="E104" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="F104" t="s">
         <v>257</v>
@@ -7647,7 +7647,7 @@
         <v>494</v>
       </c>
       <c r="E105" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="F105" t="s">
         <v>257</v>
@@ -7694,7 +7694,7 @@
         <v>412</v>
       </c>
       <c r="E106" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="F106" t="s">
         <v>257</v>
@@ -7741,7 +7741,7 @@
         <v>543</v>
       </c>
       <c r="E107" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="F107" t="s">
         <v>257</v>
@@ -7768,7 +7768,7 @@
         <v>370</v>
       </c>
       <c r="E108" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F108" t="s">
         <v>257</v>
@@ -7815,7 +7815,7 @@
         <v>375</v>
       </c>
       <c r="E109" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="F109" t="s">
         <v>257</v>
@@ -7862,7 +7862,7 @@
         <v>277</v>
       </c>
       <c r="E110" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="F110" t="s">
         <v>257</v>
@@ -7909,7 +7909,7 @@
         <v>277</v>
       </c>
       <c r="E111" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="F111" t="s">
         <v>257</v>
@@ -7956,7 +7956,7 @@
         <v>277</v>
       </c>
       <c r="E112" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="F112" t="s">
         <v>257</v>
@@ -8003,7 +8003,7 @@
         <v>893</v>
       </c>
       <c r="E113" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="F113" t="s">
         <v>261</v>
@@ -8030,7 +8030,7 @@
         <v>508</v>
       </c>
       <c r="E114" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F114" t="s">
         <v>261</v>
@@ -8077,7 +8077,7 @@
         <v>504</v>
       </c>
       <c r="E115" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F115" t="s">
         <v>257</v>
@@ -8104,7 +8104,7 @@
         <v>370</v>
       </c>
       <c r="E116" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F116" t="s">
         <v>257</v>
@@ -8151,7 +8151,7 @@
         <v>359</v>
       </c>
       <c r="E117" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F117" t="s">
         <v>261</v>
@@ -8198,7 +8198,7 @@
         <v>416</v>
       </c>
       <c r="E118" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="F118" t="s">
         <v>257</v>
@@ -8245,7 +8245,7 @@
         <v>504</v>
       </c>
       <c r="E119" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F119" t="s">
         <v>257</v>
@@ -8272,7 +8272,7 @@
         <v>365</v>
       </c>
       <c r="E120" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F120" t="s">
         <v>257</v>
@@ -8319,7 +8319,7 @@
         <v>370</v>
       </c>
       <c r="E121" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F121" t="s">
         <v>257</v>
@@ -8366,7 +8366,7 @@
         <v>271</v>
       </c>
       <c r="E122" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="F122" t="s">
         <v>257</v>
@@ -8413,7 +8413,7 @@
         <v>504</v>
       </c>
       <c r="E123" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F123" t="s">
         <v>257</v>
@@ -8460,7 +8460,7 @@
         <v>504</v>
       </c>
       <c r="E124" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F124" t="s">
         <v>257</v>
@@ -8507,7 +8507,7 @@
         <v>767</v>
       </c>
       <c r="E125" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="F125" t="s">
         <v>261</v>
@@ -8534,7 +8534,7 @@
         <v>538</v>
       </c>
       <c r="E126" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="F126" t="s">
         <v>261</v>
@@ -8581,7 +8581,7 @@
         <v>416</v>
       </c>
       <c r="E127" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="F127" t="s">
         <v>257</v>
@@ -8628,7 +8628,7 @@
         <v>370</v>
       </c>
       <c r="E128" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F128" t="s">
         <v>257</v>
@@ -8675,7 +8675,7 @@
         <v>416</v>
       </c>
       <c r="E129" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="F129" t="s">
         <v>257</v>
@@ -8702,7 +8702,7 @@
         <v>548</v>
       </c>
       <c r="E130" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="F130" t="s">
         <v>257</v>
@@ -8749,7 +8749,7 @@
         <v>340</v>
       </c>
       <c r="E131" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="F131" t="s">
         <v>261</v>
@@ -8796,7 +8796,7 @@
         <v>548</v>
       </c>
       <c r="E132" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="F132" t="s">
         <v>257</v>
@@ -8843,7 +8843,7 @@
         <v>293</v>
       </c>
       <c r="E133" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="F133" t="s">
         <v>257</v>
@@ -8890,7 +8890,7 @@
         <v>412</v>
       </c>
       <c r="E134" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="F134" t="s">
         <v>257</v>
@@ -8937,7 +8937,7 @@
         <v>312</v>
       </c>
       <c r="E135" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F135" t="s">
         <v>257</v>
@@ -8984,7 +8984,7 @@
         <v>416</v>
       </c>
       <c r="E136" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="F136" t="s">
         <v>257</v>
@@ -9011,7 +9011,7 @@
         <v>546</v>
       </c>
       <c r="E137" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="F137" t="s">
         <v>257</v>
@@ -9038,7 +9038,7 @@
         <v>416</v>
       </c>
       <c r="E138" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="F138" t="s">
         <v>257</v>
@@ -9065,7 +9065,7 @@
         <v>543</v>
       </c>
       <c r="E139" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="F139" t="s">
         <v>257</v>
@@ -9112,7 +9112,7 @@
         <v>331</v>
       </c>
       <c r="E140" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="F140" t="s">
         <v>257</v>
@@ -9159,7 +9159,7 @@
         <v>533</v>
       </c>
       <c r="E141" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="F141" t="s">
         <v>257</v>
@@ -9206,7 +9206,7 @@
         <v>504</v>
       </c>
       <c r="E142" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F142" t="s">
         <v>257</v>
@@ -9253,7 +9253,7 @@
         <v>416</v>
       </c>
       <c r="E143" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="F143" t="s">
         <v>257</v>
@@ -9300,7 +9300,7 @@
         <v>277</v>
       </c>
       <c r="E144" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="F144" t="s">
         <v>257</v>
@@ -9327,7 +9327,7 @@
         <v>298</v>
       </c>
       <c r="E145" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="F145" t="s">
         <v>261</v>
@@ -9374,7 +9374,7 @@
         <v>896</v>
       </c>
       <c r="E146" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="F146" t="s">
         <v>261</v>
@@ -9401,7 +9401,7 @@
         <v>902</v>
       </c>
       <c r="E147" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="F147" t="s">
         <v>261</v>
@@ -9428,7 +9428,7 @@
         <v>306</v>
       </c>
       <c r="E148" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="F148" t="s">
         <v>257</v>
@@ -9475,7 +9475,7 @@
         <v>291</v>
       </c>
       <c r="E149" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="F149" t="s">
         <v>261</v>
@@ -9522,7 +9522,7 @@
         <v>301</v>
       </c>
       <c r="E150" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="F150" t="s">
         <v>261</v>
@@ -9569,7 +9569,7 @@
         <v>546</v>
       </c>
       <c r="E151" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="F151" t="s">
         <v>257</v>
@@ -9596,7 +9596,7 @@
         <v>504</v>
       </c>
       <c r="E152" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F152" t="s">
         <v>257</v>
@@ -9643,7 +9643,7 @@
         <v>416</v>
       </c>
       <c r="E153" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="F153" t="s">
         <v>257</v>
@@ -9690,7 +9690,7 @@
         <v>416</v>
       </c>
       <c r="E154" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="F154" t="s">
         <v>257</v>
@@ -9717,7 +9717,7 @@
         <v>416</v>
       </c>
       <c r="E155" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="F155" t="s">
         <v>257</v>
@@ -9764,7 +9764,7 @@
         <v>407</v>
       </c>
       <c r="E156" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="F156" t="s">
         <v>257</v>
@@ -9811,7 +9811,7 @@
         <v>416</v>
       </c>
       <c r="E157" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="F157" t="s">
         <v>257</v>
@@ -9858,7 +9858,7 @@
         <v>370</v>
       </c>
       <c r="E158" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F158" t="s">
         <v>257</v>
@@ -9905,7 +9905,7 @@
         <v>407</v>
       </c>
       <c r="E159" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="F159" t="s">
         <v>257</v>
@@ -9932,7 +9932,7 @@
         <v>407</v>
       </c>
       <c r="E160" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="F160" t="s">
         <v>257</v>
@@ -9979,7 +9979,7 @@
         <v>416</v>
       </c>
       <c r="E161" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="F161" t="s">
         <v>257</v>
@@ -10006,7 +10006,7 @@
         <v>370</v>
       </c>
       <c r="E162" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F162" t="s">
         <v>257</v>
@@ -10053,7 +10053,7 @@
         <v>370</v>
       </c>
       <c r="E163" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F163" t="s">
         <v>257</v>
@@ -10100,7 +10100,7 @@
         <v>736</v>
       </c>
       <c r="E164" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="F164" t="s">
         <v>257</v>
@@ -10127,7 +10127,7 @@
         <v>894</v>
       </c>
       <c r="E165" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="F165" t="s">
         <v>261</v>
@@ -10154,7 +10154,7 @@
         <v>548</v>
       </c>
       <c r="E166" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="F166" t="s">
         <v>257</v>
@@ -10181,7 +10181,7 @@
         <v>344</v>
       </c>
       <c r="E167" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F167" t="s">
         <v>257</v>
@@ -10228,7 +10228,7 @@
         <v>502</v>
       </c>
       <c r="E168" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="F168" t="s">
         <v>257</v>
@@ -10275,7 +10275,7 @@
         <v>407</v>
       </c>
       <c r="E169" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="F169" t="s">
         <v>257</v>
@@ -10322,7 +10322,7 @@
         <v>349</v>
       </c>
       <c r="E170" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F170" t="s">
         <v>257</v>
@@ -10349,7 +10349,7 @@
         <v>560</v>
       </c>
       <c r="E171" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="F171" t="s">
         <v>261</v>
@@ -10396,7 +10396,7 @@
         <v>378</v>
       </c>
       <c r="E172" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="F172" t="s">
         <v>257</v>
@@ -10443,7 +10443,7 @@
         <v>344</v>
       </c>
       <c r="E173" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F173" t="s">
         <v>257</v>
@@ -10490,7 +10490,7 @@
         <v>344</v>
       </c>
       <c r="E174" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F174" t="s">
         <v>257</v>
@@ -10537,7 +10537,7 @@
         <v>344</v>
       </c>
       <c r="E175" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F175" t="s">
         <v>257</v>
@@ -10584,7 +10584,7 @@
         <v>344</v>
       </c>
       <c r="E176" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F176" t="s">
         <v>257</v>
@@ -10631,7 +10631,7 @@
         <v>299</v>
       </c>
       <c r="E177" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="F177" t="s">
         <v>261</v>
@@ -10678,7 +10678,7 @@
         <v>283</v>
       </c>
       <c r="E178" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="F178" t="s">
         <v>261</v>
@@ -10725,7 +10725,7 @@
         <v>429</v>
       </c>
       <c r="E179" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F179" t="s">
         <v>257</v>
@@ -10772,7 +10772,7 @@
         <v>344</v>
       </c>
       <c r="E180" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F180" t="s">
         <v>257</v>
@@ -10819,7 +10819,7 @@
         <v>354</v>
       </c>
       <c r="E181" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F181" t="s">
         <v>257</v>
@@ -10866,7 +10866,7 @@
         <v>431</v>
       </c>
       <c r="E182" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="F182" t="s">
         <v>261</v>
@@ -10913,7 +10913,7 @@
         <v>543</v>
       </c>
       <c r="E183" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="F183" t="s">
         <v>257</v>
@@ -10940,7 +10940,7 @@
         <v>543</v>
       </c>
       <c r="E184" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="F184" t="s">
         <v>257</v>
@@ -10967,7 +10967,7 @@
         <v>312</v>
       </c>
       <c r="E185" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F185" t="s">
         <v>257</v>
@@ -11014,7 +11014,7 @@
         <v>407</v>
       </c>
       <c r="E186" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="F186" t="s">
         <v>257</v>
@@ -11061,7 +11061,7 @@
         <v>370</v>
       </c>
       <c r="E187" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F187" t="s">
         <v>257</v>
@@ -11108,7 +11108,7 @@
         <v>312</v>
       </c>
       <c r="E188" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F188" t="s">
         <v>257</v>
@@ -11155,7 +11155,7 @@
         <v>310</v>
       </c>
       <c r="E189" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F189" t="s">
         <v>261</v>
@@ -11202,7 +11202,7 @@
         <v>419</v>
       </c>
       <c r="E190" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F190" t="s">
         <v>257</v>
@@ -11229,7 +11229,7 @@
         <v>370</v>
       </c>
       <c r="E191" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F191" t="s">
         <v>257</v>
@@ -11276,7 +11276,7 @@
         <v>754</v>
       </c>
       <c r="E192" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="F192" t="s">
         <v>257</v>
@@ -11303,7 +11303,7 @@
         <v>344</v>
       </c>
       <c r="E193" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F193" t="s">
         <v>257</v>
@@ -11330,7 +11330,7 @@
         <v>365</v>
       </c>
       <c r="E194" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F194" t="s">
         <v>257</v>
@@ -11357,7 +11357,7 @@
         <v>541</v>
       </c>
       <c r="E195" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="F195" t="s">
         <v>261</v>
@@ -11404,7 +11404,7 @@
         <v>312</v>
       </c>
       <c r="E196" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F196" t="s">
         <v>257</v>
@@ -11451,7 +11451,7 @@
         <v>344</v>
       </c>
       <c r="E197" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F197" t="s">
         <v>257</v>
@@ -11498,7 +11498,7 @@
         <v>354</v>
       </c>
       <c r="E198" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F198" t="s">
         <v>257</v>
@@ -11545,7 +11545,7 @@
         <v>344</v>
       </c>
       <c r="E199" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F199" t="s">
         <v>257</v>
@@ -11592,7 +11592,7 @@
         <v>546</v>
       </c>
       <c r="E200" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="F200" t="s">
         <v>257</v>
@@ -11619,7 +11619,7 @@
         <v>344</v>
       </c>
       <c r="E201" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F201" t="s">
         <v>257</v>
@@ -11666,7 +11666,7 @@
         <v>344</v>
       </c>
       <c r="E202" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F202" t="s">
         <v>257</v>
@@ -11693,7 +11693,7 @@
         <v>344</v>
       </c>
       <c r="E203" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F203" t="s">
         <v>257</v>
@@ -11720,7 +11720,7 @@
         <v>344</v>
       </c>
       <c r="E204" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F204" t="s">
         <v>257</v>
@@ -11767,7 +11767,7 @@
         <v>543</v>
       </c>
       <c r="E205" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="F205" t="s">
         <v>257</v>
@@ -11814,7 +11814,7 @@
         <v>312</v>
       </c>
       <c r="E206" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F206" t="s">
         <v>257</v>
@@ -11861,7 +11861,7 @@
         <v>290</v>
       </c>
       <c r="E207" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="F207" t="s">
         <v>257</v>
@@ -11908,7 +11908,7 @@
         <v>546</v>
       </c>
       <c r="E208" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="F208" t="s">
         <v>257</v>
@@ -11955,7 +11955,7 @@
         <v>370</v>
       </c>
       <c r="E209" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F209" t="s">
         <v>257</v>
@@ -12002,7 +12002,7 @@
         <v>502</v>
       </c>
       <c r="E210" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="F210" t="s">
         <v>257</v>
@@ -12049,7 +12049,7 @@
         <v>288</v>
       </c>
       <c r="E211" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="F211" t="s">
         <v>261</v>
@@ -12096,7 +12096,7 @@
         <v>267</v>
       </c>
       <c r="E212" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="F212" t="s">
         <v>261</v>
@@ -12143,7 +12143,7 @@
         <v>370</v>
       </c>
       <c r="E213" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F213" t="s">
         <v>257</v>
@@ -12190,7 +12190,7 @@
         <v>349</v>
       </c>
       <c r="E214" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F214" t="s">
         <v>257</v>
@@ -12237,7 +12237,7 @@
         <v>370</v>
       </c>
       <c r="E215" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F215" t="s">
         <v>257</v>
@@ -12284,7 +12284,7 @@
         <v>494</v>
       </c>
       <c r="E216" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="F216" t="s">
         <v>257</v>
@@ -12331,7 +12331,7 @@
         <v>530</v>
       </c>
       <c r="E217" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="F217" t="s">
         <v>261</v>
@@ -12378,7 +12378,7 @@
         <v>421</v>
       </c>
       <c r="E218" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="F218" t="s">
         <v>257</v>
@@ -12425,7 +12425,7 @@
         <v>344</v>
       </c>
       <c r="E219" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F219" t="s">
         <v>257</v>
@@ -12472,7 +12472,7 @@
         <v>329</v>
       </c>
       <c r="E220" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="F220" t="s">
         <v>261</v>
@@ -12519,7 +12519,7 @@
         <v>536</v>
       </c>
       <c r="E221" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="F221" t="s">
         <v>257</v>
@@ -12566,7 +12566,7 @@
         <v>742</v>
       </c>
       <c r="E222" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F222" t="s">
         <v>257</v>
@@ -12593,7 +12593,7 @@
         <v>452</v>
       </c>
       <c r="E223" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="F223" t="s">
         <v>257</v>
@@ -12640,7 +12640,7 @@
         <v>494</v>
       </c>
       <c r="E224" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="F224" t="s">
         <v>257</v>
@@ -12687,7 +12687,7 @@
         <v>412</v>
       </c>
       <c r="E225" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="F225" t="s">
         <v>257</v>
@@ -12734,7 +12734,7 @@
         <v>344</v>
       </c>
       <c r="E226" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F226" t="s">
         <v>257</v>
@@ -12781,7 +12781,7 @@
         <v>518</v>
       </c>
       <c r="E227" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F227" t="s">
         <v>257</v>
@@ -12828,7 +12828,7 @@
         <v>354</v>
       </c>
       <c r="E228" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F228" t="s">
         <v>257</v>
@@ -12875,7 +12875,7 @@
         <v>419</v>
       </c>
       <c r="E229" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F229" t="s">
         <v>257</v>
@@ -12902,7 +12902,7 @@
         <v>419</v>
       </c>
       <c r="E230" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F230" t="s">
         <v>257</v>
@@ -12929,7 +12929,7 @@
         <v>419</v>
       </c>
       <c r="E231" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F231" t="s">
         <v>257</v>
@@ -12956,7 +12956,7 @@
         <v>419</v>
       </c>
       <c r="E232" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F232" t="s">
         <v>257</v>
@@ -12983,7 +12983,7 @@
         <v>419</v>
       </c>
       <c r="E233" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F233" t="s">
         <v>257</v>
@@ -13010,7 +13010,7 @@
         <v>419</v>
       </c>
       <c r="E234" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F234" t="s">
         <v>257</v>
@@ -13037,7 +13037,7 @@
         <v>256</v>
       </c>
       <c r="E235" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F235" t="s">
         <v>257</v>
@@ -13084,7 +13084,7 @@
         <v>256</v>
       </c>
       <c r="E236" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F236" t="s">
         <v>257</v>
@@ -13131,7 +13131,7 @@
         <v>370</v>
       </c>
       <c r="E237" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F237" t="s">
         <v>257</v>
@@ -13158,7 +13158,7 @@
         <v>407</v>
       </c>
       <c r="E238" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="F238" t="s">
         <v>257</v>
@@ -13205,7 +13205,7 @@
         <v>370</v>
       </c>
       <c r="E239" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F239" t="s">
         <v>257</v>
@@ -13232,7 +13232,7 @@
         <v>370</v>
       </c>
       <c r="E240" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F240" t="s">
         <v>257</v>
@@ -13279,7 +13279,7 @@
         <v>370</v>
       </c>
       <c r="E241" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F241" t="s">
         <v>257</v>
@@ -13306,7 +13306,7 @@
         <v>370</v>
       </c>
       <c r="E242" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F242" t="s">
         <v>257</v>
@@ -13333,7 +13333,7 @@
         <v>370</v>
       </c>
       <c r="E243" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F243" t="s">
         <v>257</v>
@@ -13380,7 +13380,7 @@
         <v>370</v>
       </c>
       <c r="E244" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F244" t="s">
         <v>257</v>
@@ -13427,7 +13427,7 @@
         <v>407</v>
       </c>
       <c r="E245" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="F245" t="s">
         <v>257</v>
@@ -13474,7 +13474,7 @@
         <v>370</v>
       </c>
       <c r="E246" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F246" t="s">
         <v>257</v>
@@ -13521,7 +13521,7 @@
         <v>370</v>
       </c>
       <c r="E247" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F247" t="s">
         <v>257</v>
@@ -13568,7 +13568,7 @@
         <v>370</v>
       </c>
       <c r="E248" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F248" t="s">
         <v>257</v>
@@ -13615,7 +13615,7 @@
         <v>304</v>
       </c>
       <c r="E249" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="F249" t="s">
         <v>261</v>
@@ -13662,7 +13662,7 @@
         <v>407</v>
       </c>
       <c r="E250" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="F250" t="s">
         <v>257</v>
@@ -13689,7 +13689,7 @@
         <v>370</v>
       </c>
       <c r="E251" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F251" t="s">
         <v>257</v>
@@ -13736,7 +13736,7 @@
         <v>370</v>
       </c>
       <c r="E252" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F252" t="s">
         <v>257</v>
@@ -13763,7 +13763,7 @@
         <v>370</v>
       </c>
       <c r="E253" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F253" t="s">
         <v>257</v>
@@ -13790,7 +13790,7 @@
         <v>494</v>
       </c>
       <c r="E254" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="F254" t="s">
         <v>257</v>
@@ -13837,7 +13837,7 @@
         <v>410</v>
       </c>
       <c r="E255" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="F255" t="s">
         <v>257</v>
@@ -13884,7 +13884,7 @@
         <v>327</v>
       </c>
       <c r="E256" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="F256" t="s">
         <v>261</v>
@@ -13931,7 +13931,7 @@
         <v>752</v>
       </c>
       <c r="E257" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F257" t="s">
         <v>261</v>
@@ -13958,7 +13958,7 @@
         <v>344</v>
       </c>
       <c r="E258" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F258" t="s">
         <v>257</v>
@@ -14005,7 +14005,7 @@
         <v>546</v>
       </c>
       <c r="E259" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="F259" t="s">
         <v>257</v>
@@ -14032,7 +14032,7 @@
         <v>344</v>
       </c>
       <c r="E260" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F260" t="s">
         <v>257</v>
@@ -14079,7 +14079,7 @@
         <v>414</v>
       </c>
       <c r="E261" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="F261" t="s">
         <v>261</v>
@@ -14126,7 +14126,7 @@
         <v>370</v>
       </c>
       <c r="E262" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F262" t="s">
         <v>257</v>
@@ -14153,7 +14153,7 @@
         <v>462</v>
       </c>
       <c r="E263" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="F263" t="s">
         <v>261</v>
@@ -14200,7 +14200,7 @@
         <v>516</v>
       </c>
       <c r="E264" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F264" t="s">
         <v>257</v>
@@ -14247,7 +14247,7 @@
         <v>407</v>
       </c>
       <c r="E265" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="F265" t="s">
         <v>257</v>
@@ -14274,7 +14274,7 @@
         <v>736</v>
       </c>
       <c r="E266" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="F266" t="s">
         <v>257</v>
@@ -14301,7 +14301,7 @@
         <v>736</v>
       </c>
       <c r="E267" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="F267" t="s">
         <v>257</v>
@@ -14328,7 +14328,7 @@
         <v>736</v>
       </c>
       <c r="E268" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="F268" t="s">
         <v>257</v>
@@ -14355,7 +14355,7 @@
         <v>308</v>
       </c>
       <c r="E269" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="F269" t="s">
         <v>257</v>
@@ -14402,7 +14402,7 @@
         <v>265</v>
       </c>
       <c r="E270" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="F270" t="s">
         <v>261</v>
@@ -14449,7 +14449,7 @@
         <v>419</v>
       </c>
       <c r="E271" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F271" t="s">
         <v>257</v>
@@ -14476,7 +14476,7 @@
         <v>419</v>
       </c>
       <c r="E272" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F272" t="s">
         <v>257</v>
@@ -14523,7 +14523,7 @@
         <v>419</v>
       </c>
       <c r="E273" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F273" t="s">
         <v>257</v>
@@ -14550,7 +14550,7 @@
         <v>419</v>
       </c>
       <c r="E274" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F274" t="s">
         <v>257</v>
@@ -14577,7 +14577,7 @@
         <v>419</v>
       </c>
       <c r="E275" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F275" t="s">
         <v>257</v>
@@ -14604,7 +14604,7 @@
         <v>419</v>
       </c>
       <c r="E276" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F276" t="s">
         <v>257</v>
@@ -14631,7 +14631,7 @@
         <v>419</v>
       </c>
       <c r="E277" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F277" t="s">
         <v>257</v>
@@ -14658,7 +14658,7 @@
         <v>419</v>
       </c>
       <c r="E278" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F278" t="s">
         <v>257</v>
@@ -14685,7 +14685,7 @@
         <v>419</v>
       </c>
       <c r="E279" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F279" t="s">
         <v>257</v>
@@ -14712,7 +14712,7 @@
         <v>419</v>
       </c>
       <c r="E280" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F280" t="s">
         <v>257</v>
@@ -14759,7 +14759,7 @@
         <v>419</v>
       </c>
       <c r="E281" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F281" t="s">
         <v>257</v>
@@ -14786,7 +14786,7 @@
         <v>419</v>
       </c>
       <c r="E282" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F282" t="s">
         <v>257</v>
@@ -14833,7 +14833,7 @@
         <v>419</v>
       </c>
       <c r="E283" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F283" t="s">
         <v>257</v>
@@ -14860,7 +14860,7 @@
         <v>419</v>
       </c>
       <c r="E284" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F284" t="s">
         <v>257</v>
@@ -14887,7 +14887,7 @@
         <v>419</v>
       </c>
       <c r="E285" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F285" t="s">
         <v>257</v>
@@ -14914,7 +14914,7 @@
         <v>419</v>
       </c>
       <c r="E286" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F286" t="s">
         <v>257</v>
@@ -14961,7 +14961,7 @@
         <v>419</v>
       </c>
       <c r="E287" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F287" t="s">
         <v>257</v>
@@ -15008,7 +15008,7 @@
         <v>419</v>
       </c>
       <c r="E288" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F288" t="s">
         <v>257</v>
@@ -15035,7 +15035,7 @@
         <v>419</v>
       </c>
       <c r="E289" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F289" t="s">
         <v>257</v>
@@ -15062,7 +15062,7 @@
         <v>419</v>
       </c>
       <c r="E290" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F290" t="s">
         <v>257</v>
@@ -15089,7 +15089,7 @@
         <v>419</v>
       </c>
       <c r="E291" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F291" t="s">
         <v>257</v>
@@ -15116,7 +15116,7 @@
         <v>419</v>
       </c>
       <c r="E292" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F292" t="s">
         <v>257</v>
@@ -15143,7 +15143,7 @@
         <v>419</v>
       </c>
       <c r="E293" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F293" t="s">
         <v>257</v>
@@ -15190,7 +15190,7 @@
         <v>419</v>
       </c>
       <c r="E294" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F294" t="s">
         <v>257</v>
@@ -15217,7 +15217,7 @@
         <v>419</v>
       </c>
       <c r="E295" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F295" t="s">
         <v>257</v>
@@ -15264,7 +15264,7 @@
         <v>419</v>
       </c>
       <c r="E296" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F296" t="s">
         <v>257</v>
@@ -15311,7 +15311,7 @@
         <v>419</v>
       </c>
       <c r="E297" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F297" t="s">
         <v>257</v>
@@ -15338,7 +15338,7 @@
         <v>419</v>
       </c>
       <c r="E298" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F298" t="s">
         <v>257</v>
@@ -15365,7 +15365,7 @@
         <v>419</v>
       </c>
       <c r="E299" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F299" t="s">
         <v>257</v>
@@ -15392,7 +15392,7 @@
         <v>419</v>
       </c>
       <c r="E300" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F300" t="s">
         <v>257</v>
@@ -15419,7 +15419,7 @@
         <v>419</v>
       </c>
       <c r="E301" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F301" t="s">
         <v>257</v>
@@ -15446,7 +15446,7 @@
         <v>419</v>
       </c>
       <c r="E302" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F302" t="s">
         <v>257</v>
@@ -15473,7 +15473,7 @@
         <v>419</v>
       </c>
       <c r="E303" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F303" t="s">
         <v>257</v>
@@ -15500,7 +15500,7 @@
         <v>419</v>
       </c>
       <c r="E304" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F304" t="s">
         <v>257</v>
@@ -15547,7 +15547,7 @@
         <v>419</v>
       </c>
       <c r="E305" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F305" t="s">
         <v>257</v>
@@ -15574,7 +15574,7 @@
         <v>419</v>
       </c>
       <c r="E306" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F306" t="s">
         <v>257</v>
@@ -15621,7 +15621,7 @@
         <v>419</v>
       </c>
       <c r="E307" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F307" t="s">
         <v>257</v>
@@ -15668,7 +15668,7 @@
         <v>419</v>
       </c>
       <c r="E308" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F308" t="s">
         <v>257</v>
@@ -15715,7 +15715,7 @@
         <v>419</v>
       </c>
       <c r="E309" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F309" t="s">
         <v>257</v>
@@ -15742,7 +15742,7 @@
         <v>419</v>
       </c>
       <c r="E310" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F310" t="s">
         <v>257</v>
@@ -15769,7 +15769,7 @@
         <v>419</v>
       </c>
       <c r="E311" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F311" t="s">
         <v>257</v>
@@ -15796,7 +15796,7 @@
         <v>419</v>
       </c>
       <c r="E312" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F312" t="s">
         <v>257</v>
@@ -15823,7 +15823,7 @@
         <v>419</v>
       </c>
       <c r="E313" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F313" t="s">
         <v>257</v>
@@ -15850,7 +15850,7 @@
         <v>419</v>
       </c>
       <c r="E314" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F314" t="s">
         <v>257</v>
@@ -15877,7 +15877,7 @@
         <v>419</v>
       </c>
       <c r="E315" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F315" t="s">
         <v>257</v>
@@ -15924,7 +15924,7 @@
         <v>419</v>
       </c>
       <c r="E316" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F316" t="s">
         <v>257</v>
@@ -15951,7 +15951,7 @@
         <v>419</v>
       </c>
       <c r="E317" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F317" t="s">
         <v>257</v>
@@ -15978,7 +15978,7 @@
         <v>419</v>
       </c>
       <c r="E318" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F318" t="s">
         <v>257</v>
@@ -16005,7 +16005,7 @@
         <v>419</v>
       </c>
       <c r="E319" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F319" t="s">
         <v>257</v>
@@ -16052,7 +16052,7 @@
         <v>419</v>
       </c>
       <c r="E320" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F320" t="s">
         <v>257</v>
@@ -16079,7 +16079,7 @@
         <v>419</v>
       </c>
       <c r="E321" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F321" t="s">
         <v>257</v>
@@ -16106,7 +16106,7 @@
         <v>419</v>
       </c>
       <c r="E322" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F322" t="s">
         <v>257</v>
@@ -16133,7 +16133,7 @@
         <v>419</v>
       </c>
       <c r="E323" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F323" t="s">
         <v>257</v>
@@ -16160,7 +16160,7 @@
         <v>419</v>
       </c>
       <c r="E324" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F324" t="s">
         <v>257</v>
@@ -16187,7 +16187,7 @@
         <v>419</v>
       </c>
       <c r="E325" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F325" t="s">
         <v>257</v>
@@ -16214,7 +16214,7 @@
         <v>419</v>
       </c>
       <c r="E326" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F326" t="s">
         <v>257</v>
@@ -16241,7 +16241,7 @@
         <v>419</v>
       </c>
       <c r="E327" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F327" t="s">
         <v>257</v>
@@ -16268,7 +16268,7 @@
         <v>419</v>
       </c>
       <c r="E328" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F328" t="s">
         <v>257</v>
@@ -16295,7 +16295,7 @@
         <v>419</v>
       </c>
       <c r="E329" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F329" t="s">
         <v>257</v>
@@ -16322,7 +16322,7 @@
         <v>419</v>
       </c>
       <c r="E330" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F330" t="s">
         <v>257</v>
@@ -16349,7 +16349,7 @@
         <v>419</v>
       </c>
       <c r="E331" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F331" t="s">
         <v>257</v>
@@ -16396,7 +16396,7 @@
         <v>419</v>
       </c>
       <c r="E332" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F332" t="s">
         <v>257</v>
@@ -16423,7 +16423,7 @@
         <v>419</v>
       </c>
       <c r="E333" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F333" t="s">
         <v>257</v>
@@ -16470,7 +16470,7 @@
         <v>419</v>
       </c>
       <c r="E334" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F334" t="s">
         <v>257</v>
@@ -16497,7 +16497,7 @@
         <v>419</v>
       </c>
       <c r="E335" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F335" t="s">
         <v>257</v>
@@ -16524,7 +16524,7 @@
         <v>419</v>
       </c>
       <c r="E336" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F336" t="s">
         <v>257</v>
@@ -16551,7 +16551,7 @@
         <v>419</v>
       </c>
       <c r="E337" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F337" t="s">
         <v>257</v>
@@ -16578,7 +16578,7 @@
         <v>419</v>
       </c>
       <c r="E338" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F338" t="s">
         <v>257</v>
@@ -16625,7 +16625,7 @@
         <v>419</v>
       </c>
       <c r="E339" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F339" t="s">
         <v>257</v>
@@ -16652,7 +16652,7 @@
         <v>419</v>
       </c>
       <c r="E340" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F340" t="s">
         <v>257</v>
@@ -16679,7 +16679,7 @@
         <v>419</v>
       </c>
       <c r="E341" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F341" t="s">
         <v>257</v>
@@ -16706,7 +16706,7 @@
         <v>419</v>
       </c>
       <c r="E342" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F342" t="s">
         <v>257</v>
@@ -16733,7 +16733,7 @@
         <v>419</v>
       </c>
       <c r="E343" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F343" t="s">
         <v>257</v>
@@ -16760,7 +16760,7 @@
         <v>419</v>
       </c>
       <c r="E344" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F344" t="s">
         <v>257</v>
@@ -16787,7 +16787,7 @@
         <v>419</v>
       </c>
       <c r="E345" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F345" t="s">
         <v>257</v>
@@ -16814,7 +16814,7 @@
         <v>419</v>
       </c>
       <c r="E346" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F346" t="s">
         <v>257</v>
@@ -16841,7 +16841,7 @@
         <v>419</v>
       </c>
       <c r="E347" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F347" t="s">
         <v>257</v>
@@ -16888,7 +16888,7 @@
         <v>419</v>
       </c>
       <c r="E348" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F348" t="s">
         <v>257</v>
@@ -16915,7 +16915,7 @@
         <v>419</v>
       </c>
       <c r="E349" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F349" t="s">
         <v>257</v>
@@ -16962,7 +16962,7 @@
         <v>419</v>
       </c>
       <c r="E350" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F350" t="s">
         <v>257</v>
@@ -16989,7 +16989,7 @@
         <v>419</v>
       </c>
       <c r="E351" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F351" t="s">
         <v>257</v>
@@ -17016,7 +17016,7 @@
         <v>419</v>
       </c>
       <c r="E352" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F352" t="s">
         <v>257</v>
@@ -17063,7 +17063,7 @@
         <v>419</v>
       </c>
       <c r="E353" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F353" t="s">
         <v>257</v>
@@ -17090,7 +17090,7 @@
         <v>419</v>
       </c>
       <c r="E354" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F354" t="s">
         <v>257</v>
@@ -17137,7 +17137,7 @@
         <v>419</v>
       </c>
       <c r="E355" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F355" t="s">
         <v>257</v>
@@ -17164,7 +17164,7 @@
         <v>419</v>
       </c>
       <c r="E356" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F356" t="s">
         <v>257</v>
@@ -17191,7 +17191,7 @@
         <v>419</v>
       </c>
       <c r="E357" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F357" t="s">
         <v>257</v>
@@ -17218,7 +17218,7 @@
         <v>419</v>
       </c>
       <c r="E358" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F358" t="s">
         <v>257</v>
@@ -17245,7 +17245,7 @@
         <v>419</v>
       </c>
       <c r="E359" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F359" t="s">
         <v>257</v>
@@ -17292,7 +17292,7 @@
         <v>419</v>
       </c>
       <c r="E360" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F360" t="s">
         <v>257</v>
@@ -17319,7 +17319,7 @@
         <v>419</v>
       </c>
       <c r="E361" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F361" t="s">
         <v>257</v>
@@ -17366,7 +17366,7 @@
         <v>419</v>
       </c>
       <c r="E362" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F362" t="s">
         <v>257</v>
@@ -17413,7 +17413,7 @@
         <v>419</v>
       </c>
       <c r="E363" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F363" t="s">
         <v>257</v>
@@ -17440,7 +17440,7 @@
         <v>419</v>
       </c>
       <c r="E364" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F364" t="s">
         <v>257</v>
@@ -17467,7 +17467,7 @@
         <v>419</v>
       </c>
       <c r="E365" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F365" t="s">
         <v>257</v>
@@ -17514,7 +17514,7 @@
         <v>419</v>
       </c>
       <c r="E366" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F366" t="s">
         <v>257</v>
@@ -17541,7 +17541,7 @@
         <v>419</v>
       </c>
       <c r="E367" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F367" t="s">
         <v>257</v>
@@ -17568,7 +17568,7 @@
         <v>419</v>
       </c>
       <c r="E368" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F368" t="s">
         <v>257</v>
@@ -17595,7 +17595,7 @@
         <v>419</v>
       </c>
       <c r="E369" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F369" t="s">
         <v>257</v>
@@ -17622,7 +17622,7 @@
         <v>419</v>
       </c>
       <c r="E370" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F370" t="s">
         <v>257</v>
@@ -17649,7 +17649,7 @@
         <v>419</v>
       </c>
       <c r="E371" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F371" t="s">
         <v>257</v>
@@ -17676,7 +17676,7 @@
         <v>419</v>
       </c>
       <c r="E372" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F372" t="s">
         <v>257</v>
@@ -17703,7 +17703,7 @@
         <v>419</v>
       </c>
       <c r="E373" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F373" t="s">
         <v>257</v>
@@ -17730,7 +17730,7 @@
         <v>419</v>
       </c>
       <c r="E374" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F374" t="s">
         <v>257</v>
@@ -17757,7 +17757,7 @@
         <v>419</v>
       </c>
       <c r="E375" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F375" t="s">
         <v>257</v>
@@ -17784,7 +17784,7 @@
         <v>419</v>
       </c>
       <c r="E376" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F376" t="s">
         <v>257</v>
@@ -17831,7 +17831,7 @@
         <v>419</v>
       </c>
       <c r="E377" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F377" t="s">
         <v>257</v>
@@ -17858,7 +17858,7 @@
         <v>419</v>
       </c>
       <c r="E378" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="F378" t="s">
         <v>257</v>
@@ -17885,7 +17885,7 @@
         <v>303</v>
       </c>
       <c r="E379" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="F379" t="s">
         <v>261</v>
@@ -17932,7 +17932,7 @@
         <v>407</v>
       </c>
       <c r="E380" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="F380" t="s">
         <v>257</v>
@@ -17979,7 +17979,7 @@
         <v>370</v>
       </c>
       <c r="E381" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F381" t="s">
         <v>257</v>
@@ -18006,7 +18006,7 @@
         <v>767</v>
       </c>
       <c r="E382" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="F382" t="s">
         <v>261</v>
@@ -18033,7 +18033,7 @@
         <v>742</v>
       </c>
       <c r="E383" t="s">
-        <v>916</v>
+        <v>946</v>
       </c>
       <c r="F383" t="s">
         <v>257</v>
@@ -18060,7 +18060,7 @@
         <v>407</v>
       </c>
       <c r="E384" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="F384" t="s">
         <v>257</v>
@@ -18087,7 +18087,7 @@
         <v>880</v>
       </c>
       <c r="E385" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="F385" t="s">
         <v>257</v>
@@ -18114,7 +18114,7 @@
         <v>452</v>
       </c>
       <c r="E386" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="F386" t="s">
         <v>257</v>
@@ -18161,7 +18161,7 @@
         <v>452</v>
       </c>
       <c r="E387" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="F387" t="s">
         <v>257</v>
@@ -18208,7 +18208,7 @@
         <v>421</v>
       </c>
       <c r="E388" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="F388" t="s">
         <v>257</v>
@@ -18255,7 +18255,7 @@
         <v>319</v>
       </c>
       <c r="E389" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="F389" t="s">
         <v>257</v>
@@ -18302,7 +18302,7 @@
         <v>319</v>
       </c>
       <c r="E390" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="F390" t="s">
         <v>257</v>
@@ -18349,7 +18349,7 @@
         <v>319</v>
       </c>
       <c r="E391" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="F391" t="s">
         <v>257</v>
@@ -18396,7 +18396,7 @@
         <v>319</v>
       </c>
       <c r="E392" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="F392" t="s">
         <v>257</v>
@@ -18443,7 +18443,7 @@
         <v>319</v>
       </c>
       <c r="E393" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="F393" t="s">
         <v>257</v>
@@ -18490,7 +18490,7 @@
         <v>319</v>
       </c>
       <c r="E394" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="F394" t="s">
         <v>257</v>
@@ -18537,7 +18537,7 @@
         <v>319</v>
       </c>
       <c r="E395" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="F395" t="s">
         <v>257</v>
@@ -18564,7 +18564,7 @@
         <v>319</v>
       </c>
       <c r="E396" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="F396" t="s">
         <v>257</v>
@@ -18591,7 +18591,7 @@
         <v>319</v>
       </c>
       <c r="E397" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="F397" t="s">
         <v>257</v>
@@ -18638,7 +18638,7 @@
         <v>319</v>
       </c>
       <c r="E398" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="F398" t="s">
         <v>257</v>
@@ -18685,7 +18685,7 @@
         <v>319</v>
       </c>
       <c r="E399" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="F399" t="s">
         <v>257</v>
@@ -18732,7 +18732,7 @@
         <v>319</v>
       </c>
       <c r="E400" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="F400" t="s">
         <v>257</v>
@@ -18779,7 +18779,7 @@
         <v>319</v>
       </c>
       <c r="E401" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="F401" t="s">
         <v>257</v>
@@ -18826,7 +18826,7 @@
         <v>319</v>
       </c>
       <c r="E402" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="F402" t="s">
         <v>257</v>
@@ -18873,7 +18873,7 @@
         <v>319</v>
       </c>
       <c r="E403" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="F403" t="s">
         <v>257</v>
@@ -18920,7 +18920,7 @@
         <v>319</v>
       </c>
       <c r="E404" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="F404" t="s">
         <v>257</v>
@@ -18967,7 +18967,7 @@
         <v>319</v>
       </c>
       <c r="E405" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="F405" t="s">
         <v>257</v>

</xml_diff>